<commit_message>
converter, model improvements, new endpoints
</commit_message>
<xml_diff>
--- a/utils/report.xlsx
+++ b/utils/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steel\OneDrive\Документы\Github\spouralExcel\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pomid\repos\spouralExcel\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B4C736-D5BB-4109-9060-8C7B5995A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258F8B66-BF93-45DA-92EC-55450916D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1035" windowWidth="20325" windowHeight="15345" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Титульный лист" sheetId="8" r:id="rId1"/>
@@ -697,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1275,10 +1275,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1465,9 +1461,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1505,7 +1501,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1611,7 +1607,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1753,7 +1749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1764,20 +1760,20 @@
   <dimension ref="A1:BW53"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A5" zoomScale="115" zoomScaleNormal="160" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q1:Q1048576"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="1" width="2.6640625" style="6"/>
+    <col min="2" max="2" width="2.6640625" style="6" customWidth="1"/>
+    <col min="3" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="35"/>
@@ -1856,7 +1852,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="37"/>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
@@ -1893,7 +1889,7 @@
       <c r="AJ2" s="72"/>
       <c r="AK2" s="73"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="37"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -1930,7 +1926,7 @@
       <c r="AJ3" s="72"/>
       <c r="AK3" s="73"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="39"/>
       <c r="D4" s="40"/>
       <c r="E4" s="38"/>
@@ -1967,7 +1963,7 @@
       <c r="AJ4" s="72"/>
       <c r="AK4" s="73"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -1975,7 +1971,7 @@
       <c r="AK5" s="12"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="78" t="s">
         <v>20</v>
@@ -2014,7 +2010,7 @@
       <c r="AJ6" s="78"/>
       <c r="AK6" s="15"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="78"/>
       <c r="E7" s="78"/>
@@ -2051,11 +2047,11 @@
       <c r="AJ7" s="78"/>
       <c r="AK7" s="15"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="77" t="s">
         <v>21</v>
@@ -2094,7 +2090,7 @@
       <c r="AJ9" s="77"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="77"/>
       <c r="E10" s="77"/>
@@ -2131,7 +2127,7 @@
       <c r="AJ10" s="77"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="77"/>
       <c r="E11" s="77"/>
@@ -2168,11 +2164,11 @@
       <c r="AJ11" s="77"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="74" t="s">
         <v>12</v>
@@ -2211,7 +2207,7 @@
       <c r="AJ13" s="74"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="74"/>
       <c r="E14" s="74"/>
@@ -2248,7 +2244,7 @@
       <c r="AJ14" s="74"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="74"/>
       <c r="E15" s="74"/>
@@ -2285,7 +2281,7 @@
       <c r="AJ15" s="74"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="74"/>
       <c r="E16" s="74"/>
@@ -2322,7 +2318,7 @@
       <c r="AJ16" s="74"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="74"/>
       <c r="E17" s="74"/>
@@ -2359,15 +2355,15 @@
       <c r="AJ17" s="74"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="79" t="s">
         <v>18</v>
@@ -2406,7 +2402,7 @@
       <c r="AJ20" s="79"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="79"/>
       <c r="E21" s="79"/>
@@ -2443,19 +2439,19 @@
       <c r="AJ21" s="79"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -2498,7 +2494,7 @@
       <c r="AJ25" s="74"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
@@ -2537,13 +2533,13 @@
       <c r="AJ26" s="74"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -2584,7 +2580,7 @@
       <c r="AJ28" s="79"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
@@ -2623,19 +2619,19 @@
       <c r="AJ29" s="79"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -2643,31 +2639,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -2675,19 +2671,19 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
@@ -2730,7 +2726,7 @@
       <c r="AJ40" s="76"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
@@ -2754,7 +2750,7 @@
       <c r="AJ41" s="76"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -2762,24 +2758,24 @@
       <c r="C42" s="7"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="12"/>
     </row>
-    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="67"/>
       <c r="C46" s="10"/>
@@ -2806,7 +2802,7 @@
       <c r="AJ46" s="26"/>
       <c r="AK46" s="27"/>
     </row>
-    <row r="47" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="67"/>
       <c r="C47" s="28"/>
@@ -2843,7 +2839,7 @@
       <c r="AJ47" s="26"/>
       <c r="AK47" s="27"/>
     </row>
-    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="68"/>
       <c r="C48" s="42"/>
@@ -2882,7 +2878,7 @@
       <c r="AJ48" s="26"/>
       <c r="AK48" s="27"/>
     </row>
-    <row r="49" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -2923,7 +2919,7 @@
       <c r="AJ49" s="14"/>
       <c r="AK49" s="15"/>
     </row>
-    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="61"/>
       <c r="B50" s="67"/>
       <c r="C50" s="28"/>
@@ -2962,7 +2958,7 @@
       <c r="AJ50" s="29"/>
       <c r="AK50" s="43"/>
     </row>
-    <row r="51" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="61"/>
       <c r="B51" s="67"/>
       <c r="C51" s="28"/>
@@ -3003,7 +2999,7 @@
       <c r="AJ51" s="69"/>
       <c r="AK51" s="43"/>
     </row>
-    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="61"/>
       <c r="B52" s="67"/>
       <c r="C52" s="28"/>
@@ -3045,7 +3041,7 @@
       <c r="AJ52" s="69"/>
       <c r="AK52" s="15"/>
     </row>
-    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="68"/>
       <c r="C53" s="30"/>
@@ -3121,19 +3117,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7FCCDD-5EAB-4EE3-8581-1153B0B05959}">
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="89" t="s">
@@ -3212,7 +3208,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
       <c r="E2" s="89"/>
@@ -3249,7 +3245,7 @@
       <c r="AJ2" s="89"/>
       <c r="AK2" s="89"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="89"/>
       <c r="D3" s="89"/>
       <c r="E3" s="89"/>
@@ -3286,7 +3282,7 @@
       <c r="AJ3" s="89"/>
       <c r="AK3" s="89"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="89"/>
       <c r="D4" s="89"/>
       <c r="E4" s="89"/>
@@ -3323,7 +3319,7 @@
       <c r="AJ4" s="89"/>
       <c r="AK4" s="89"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="90" t="s">
         <v>32</v>
       </c>
@@ -3367,7 +3363,7 @@
       <c r="AK5" s="80"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="90"/>
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
@@ -3404,7 +3400,7 @@
       <c r="AJ6" s="80"/>
       <c r="AK6" s="80"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="90"/>
       <c r="D7" s="90"/>
       <c r="E7" s="90"/>
@@ -3441,11 +3437,11 @@
       <c r="AJ7" s="80"/>
       <c r="AK7" s="80"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -3482,7 +3478,7 @@
       <c r="AJ9" s="17"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -3519,7 +3515,7 @@
       <c r="AJ10" s="17"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -3556,11 +3552,11 @@
       <c r="AJ11" s="17"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -3597,7 +3593,7 @@
       <c r="AJ13" s="21"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -3634,7 +3630,7 @@
       <c r="AJ14" s="21"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -3671,7 +3667,7 @@
       <c r="AJ15" s="21"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -3708,7 +3704,7 @@
       <c r="AJ16" s="21"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -3745,15 +3741,15 @@
       <c r="AJ17" s="21"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -3790,7 +3786,7 @@
       <c r="AJ20" s="23"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -3827,15 +3823,15 @@
       <c r="AJ21" s="23"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -3872,7 +3868,7 @@
       <c r="AJ24" s="21"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -3913,13 +3909,13 @@
       <c r="AJ25" s="21"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
@@ -3958,7 +3954,7 @@
       <c r="AJ27" s="23"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -3997,25 +3993,25 @@
       <c r="AJ28" s="23"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -4023,31 +4019,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -4055,13 +4051,13 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
@@ -4096,7 +4092,7 @@
       <c r="AG39" s="25"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
@@ -4131,7 +4127,7 @@
       <c r="AG40" s="25"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
@@ -4166,7 +4162,7 @@
       <c r="AG41" s="25"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -4203,7 +4199,7 @@
       <c r="AG42" s="25"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
@@ -4242,7 +4238,7 @@
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
@@ -4281,12 +4277,12 @@
       <c r="AJ44" s="8"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="24"/>
     </row>
-    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="64"/>
       <c r="C46" s="100"/>
@@ -4327,7 +4323,7 @@
       <c r="AJ46" s="106"/>
       <c r="AK46" s="107"/>
     </row>
-    <row r="47" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="61"/>
       <c r="B47" s="64"/>
       <c r="C47" s="96"/>
@@ -4366,7 +4362,7 @@
       <c r="AJ47" s="109"/>
       <c r="AK47" s="110"/>
     </row>
-    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="65"/>
       <c r="C48" s="99" t="s">
@@ -4417,7 +4413,7 @@
       <c r="AJ48" s="112"/>
       <c r="AK48" s="113"/>
     </row>
-    <row r="49" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -4472,7 +4468,7 @@
       <c r="AJ49" s="137"/>
       <c r="AK49" s="138"/>
     </row>
-    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="61"/>
       <c r="B50" s="64"/>
       <c r="C50" s="120"/>
@@ -4513,7 +4509,7 @@
       <c r="AJ50" s="115"/>
       <c r="AK50" s="116"/>
     </row>
-    <row r="51" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="120"/>
@@ -4552,7 +4548,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="120" t="s">
@@ -4599,7 +4595,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="144" t="s">
@@ -4720,21 +4716,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95880E5D-F500-3242-A423-888689946DB1}">
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="1" width="2.6640625" style="6"/>
+    <col min="2" max="2" width="2.6640625" style="6" customWidth="1"/>
+    <col min="3" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="89" t="s">
@@ -4813,7 +4809,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
       <c r="E2" s="89"/>
@@ -4850,7 +4846,7 @@
       <c r="AJ2" s="89"/>
       <c r="AK2" s="89"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="89"/>
       <c r="D3" s="89"/>
       <c r="E3" s="89"/>
@@ -4887,7 +4883,7 @@
       <c r="AJ3" s="89"/>
       <c r="AK3" s="89"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="89"/>
       <c r="D4" s="89"/>
       <c r="E4" s="89"/>
@@ -4924,14 +4920,14 @@
       <c r="AJ4" s="89"/>
       <c r="AK4" s="89"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="AK5" s="12"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="169" t="s">
         <v>34</v>
@@ -4970,7 +4966,7 @@
       <c r="AJ6" s="169"/>
       <c r="AK6" s="15"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="169"/>
       <c r="E7" s="169"/>
@@ -5007,7 +5003,7 @@
       <c r="AJ7" s="169"/>
       <c r="AK7" s="15"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="D8" s="169"/>
       <c r="E8" s="169"/>
@@ -5044,7 +5040,7 @@
       <c r="AJ8" s="169"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="169"/>
       <c r="E9" s="169"/>
@@ -5081,7 +5077,7 @@
       <c r="AJ9" s="169"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="169"/>
       <c r="E10" s="169"/>
@@ -5118,7 +5114,7 @@
       <c r="AJ10" s="169"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="169"/>
       <c r="E11" s="169"/>
@@ -5155,7 +5151,7 @@
       <c r="AJ11" s="169"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="D12" s="169"/>
       <c r="E12" s="169"/>
@@ -5192,7 +5188,7 @@
       <c r="AJ12" s="169"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="46"/>
       <c r="E13" s="46"/>
@@ -5229,7 +5225,7 @@
       <c r="AJ13" s="46"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="46"/>
       <c r="E14" s="46"/>
@@ -5266,7 +5262,7 @@
       <c r="AJ14" s="46"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="46"/>
       <c r="E15" s="46"/>
@@ -5303,7 +5299,7 @@
       <c r="AJ15" s="46"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -5340,7 +5336,7 @@
       <c r="AJ16" s="21"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -5377,7 +5373,7 @@
       <c r="AJ17" s="21"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="D18" s="75" t="s">
         <v>35</v>
@@ -5418,11 +5414,11 @@
       <c r="AJ18" s="76"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -5459,7 +5455,7 @@
       <c r="AJ20" s="23"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -5496,15 +5492,15 @@
       <c r="AJ21" s="23"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5541,7 +5537,7 @@
       <c r="AJ24" s="21"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -5582,13 +5578,13 @@
       <c r="AJ25" s="21"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
@@ -5627,7 +5623,7 @@
       <c r="AJ27" s="23"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -5666,25 +5662,25 @@
       <c r="AJ28" s="23"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -5692,31 +5688,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -5724,31 +5720,31 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -5756,7 +5752,7 @@
       <c r="C42" s="7"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
@@ -5795,7 +5791,7 @@
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
@@ -5834,12 +5830,12 @@
       <c r="AJ44" s="8"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="12"/>
     </row>
-    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="67"/>
       <c r="C46" s="10"/>
@@ -5866,7 +5862,7 @@
       <c r="AJ46" s="26"/>
       <c r="AK46" s="27"/>
     </row>
-    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="67"/>
       <c r="C47" s="28"/>
@@ -5903,7 +5899,7 @@
       <c r="AJ47" s="26"/>
       <c r="AK47" s="27"/>
     </row>
-    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="68"/>
       <c r="C48" s="10"/>
@@ -5930,7 +5926,7 @@
       <c r="AJ48" s="26"/>
       <c r="AK48" s="27"/>
     </row>
-    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -5971,7 +5967,7 @@
       <c r="AJ49" s="14"/>
       <c r="AK49" s="15"/>
     </row>
-    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="67"/>
       <c r="C50" s="30"/>
@@ -6010,7 +6006,7 @@
       <c r="AJ50" s="33"/>
       <c r="AK50" s="34"/>
     </row>
-    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="164"/>
@@ -6053,7 +6049,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="103"/>
@@ -6092,7 +6088,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="99" t="s">
@@ -6192,20 +6188,20 @@
   <dimension ref="A1:BW53"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AN11" sqref="AN11"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="1" width="2.6640625" style="6"/>
+    <col min="2" max="2" width="2.6640625" style="6" customWidth="1"/>
+    <col min="3" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="197" t="s">
@@ -6284,7 +6280,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="197"/>
       <c r="D2" s="197"/>
       <c r="E2" s="197"/>
@@ -6321,7 +6317,7 @@
       <c r="AJ2" s="197"/>
       <c r="AK2" s="197"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="197"/>
       <c r="D3" s="197"/>
       <c r="E3" s="197"/>
@@ -6358,7 +6354,7 @@
       <c r="AJ3" s="197"/>
       <c r="AK3" s="197"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="197"/>
       <c r="D4" s="197"/>
       <c r="E4" s="197"/>
@@ -6395,7 +6391,7 @@
       <c r="AJ4" s="197"/>
       <c r="AK4" s="197"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="198" t="s">
         <v>39</v>
       </c>
@@ -6437,7 +6433,7 @@
       <c r="AK5" s="200"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="173"/>
       <c r="D6" s="174"/>
       <c r="E6" s="174"/>
@@ -6474,7 +6470,7 @@
       <c r="AJ6" s="174"/>
       <c r="AK6" s="175"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="176"/>
       <c r="D7" s="177"/>
       <c r="E7" s="177"/>
@@ -6511,7 +6507,7 @@
       <c r="AJ7" s="174"/>
       <c r="AK7" s="175"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="170" t="s">
         <v>40</v>
       </c>
@@ -6552,7 +6548,7 @@
       <c r="AJ8" s="171"/>
       <c r="AK8" s="172"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="176"/>
       <c r="D9" s="177"/>
       <c r="E9" s="177"/>
@@ -6589,7 +6585,7 @@
       <c r="AJ9" s="177"/>
       <c r="AK9" s="178"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="173" t="s">
         <v>41</v>
@@ -6630,9 +6626,8 @@
       <c r="AI10" s="171"/>
       <c r="AJ10" s="171"/>
       <c r="AK10" s="172"/>
-      <c r="AL10" s="202"/>
-    </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="173"/>
       <c r="D11" s="174"/>
@@ -6652,26 +6647,25 @@
       <c r="R11" s="174"/>
       <c r="S11" s="175"/>
       <c r="T11" s="173"/>
-      <c r="U11" s="201"/>
-      <c r="V11" s="201"/>
-      <c r="W11" s="201"/>
-      <c r="X11" s="201"/>
-      <c r="Y11" s="201"/>
-      <c r="Z11" s="201"/>
-      <c r="AA11" s="201"/>
-      <c r="AB11" s="201"/>
-      <c r="AC11" s="201"/>
-      <c r="AD11" s="201"/>
-      <c r="AE11" s="201"/>
-      <c r="AF11" s="201"/>
-      <c r="AG11" s="201"/>
-      <c r="AH11" s="201"/>
-      <c r="AI11" s="201"/>
-      <c r="AJ11" s="201"/>
+      <c r="U11" s="174"/>
+      <c r="V11" s="174"/>
+      <c r="W11" s="174"/>
+      <c r="X11" s="174"/>
+      <c r="Y11" s="174"/>
+      <c r="Z11" s="174"/>
+      <c r="AA11" s="174"/>
+      <c r="AB11" s="174"/>
+      <c r="AC11" s="174"/>
+      <c r="AD11" s="174"/>
+      <c r="AE11" s="174"/>
+      <c r="AF11" s="174"/>
+      <c r="AG11" s="174"/>
+      <c r="AH11" s="174"/>
+      <c r="AI11" s="174"/>
+      <c r="AJ11" s="174"/>
       <c r="AK11" s="175"/>
-      <c r="AL11" s="202"/>
-    </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="176"/>
       <c r="D12" s="177"/>
       <c r="E12" s="177"/>
@@ -6707,9 +6701,8 @@
       <c r="AI12" s="177"/>
       <c r="AJ12" s="177"/>
       <c r="AK12" s="178"/>
-      <c r="AL12" s="202"/>
-    </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="173" t="s">
         <v>44</v>
       </c>
@@ -6749,9 +6742,8 @@
       <c r="AI13" s="171"/>
       <c r="AJ13" s="171"/>
       <c r="AK13" s="172"/>
-      <c r="AL13" s="202"/>
-    </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="173"/>
       <c r="D14" s="174"/>
       <c r="E14" s="174"/>
@@ -6770,25 +6762,25 @@
       <c r="R14" s="174"/>
       <c r="S14" s="175"/>
       <c r="T14" s="173"/>
-      <c r="U14" s="201"/>
-      <c r="V14" s="201"/>
-      <c r="W14" s="201"/>
-      <c r="X14" s="201"/>
-      <c r="Y14" s="201"/>
-      <c r="Z14" s="201"/>
-      <c r="AA14" s="201"/>
-      <c r="AB14" s="201"/>
-      <c r="AC14" s="201"/>
-      <c r="AD14" s="201"/>
-      <c r="AE14" s="201"/>
-      <c r="AF14" s="201"/>
-      <c r="AG14" s="201"/>
-      <c r="AH14" s="201"/>
-      <c r="AI14" s="201"/>
-      <c r="AJ14" s="201"/>
+      <c r="U14" s="174"/>
+      <c r="V14" s="174"/>
+      <c r="W14" s="174"/>
+      <c r="X14" s="174"/>
+      <c r="Y14" s="174"/>
+      <c r="Z14" s="174"/>
+      <c r="AA14" s="174"/>
+      <c r="AB14" s="174"/>
+      <c r="AC14" s="174"/>
+      <c r="AD14" s="174"/>
+      <c r="AE14" s="174"/>
+      <c r="AF14" s="174"/>
+      <c r="AG14" s="174"/>
+      <c r="AH14" s="174"/>
+      <c r="AI14" s="174"/>
+      <c r="AJ14" s="174"/>
       <c r="AK14" s="175"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="173"/>
       <c r="D15" s="174"/>
       <c r="E15" s="174"/>
@@ -6825,7 +6817,7 @@
       <c r="AJ15" s="177"/>
       <c r="AK15" s="178"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="170" t="s">
         <v>45</v>
       </c>
@@ -6866,7 +6858,7 @@
       <c r="AJ16" s="183"/>
       <c r="AK16" s="184"/>
     </row>
-    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="176"/>
       <c r="D17" s="177"/>
       <c r="E17" s="177"/>
@@ -6903,7 +6895,7 @@
       <c r="AJ17" s="186"/>
       <c r="AK17" s="187"/>
     </row>
-    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="173" t="s">
         <v>46</v>
@@ -6945,7 +6937,7 @@
       <c r="AJ18" s="171"/>
       <c r="AK18" s="172"/>
     </row>
-    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="173"/>
       <c r="D19" s="174"/>
@@ -6983,7 +6975,7 @@
       <c r="AJ19" s="174"/>
       <c r="AK19" s="175"/>
     </row>
-    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="173"/>
       <c r="D20" s="174"/>
@@ -7021,7 +7013,7 @@
       <c r="AJ20" s="177"/>
       <c r="AK20" s="178"/>
     </row>
-    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="170" t="s">
         <v>47</v>
       </c>
@@ -7062,7 +7054,7 @@
       <c r="AJ21" s="189"/>
       <c r="AK21" s="190"/>
     </row>
-    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="173"/>
       <c r="D22" s="174"/>
       <c r="E22" s="174"/>
@@ -7099,7 +7091,7 @@
       <c r="AJ22" s="192"/>
       <c r="AK22" s="193"/>
     </row>
-    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="176"/>
       <c r="D23" s="177"/>
       <c r="E23" s="177"/>
@@ -7136,7 +7128,7 @@
       <c r="AJ23" s="195"/>
       <c r="AK23" s="196"/>
     </row>
-    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="170" t="s">
         <v>48</v>
       </c>
@@ -7177,7 +7169,7 @@
       <c r="AJ24" s="189"/>
       <c r="AK24" s="190"/>
     </row>
-    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -7218,7 +7210,7 @@
       <c r="AJ25" s="195"/>
       <c r="AK25" s="196"/>
     </row>
-    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="170" t="s">
@@ -7261,7 +7253,7 @@
       <c r="AJ26" s="171"/>
       <c r="AK26" s="172"/>
     </row>
-    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="173"/>
@@ -7300,7 +7292,7 @@
       <c r="AJ27" s="174"/>
       <c r="AK27" s="175"/>
     </row>
-    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="176"/>
@@ -7339,7 +7331,7 @@
       <c r="AJ28" s="177"/>
       <c r="AK28" s="178"/>
     </row>
-    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="170" t="s">
@@ -7382,7 +7374,7 @@
       <c r="AJ29" s="171"/>
       <c r="AK29" s="172"/>
     </row>
-    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="176"/>
@@ -7421,7 +7413,7 @@
       <c r="AJ30" s="177"/>
       <c r="AK30" s="178"/>
     </row>
-    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="170" t="s">
@@ -7464,7 +7456,7 @@
       <c r="AJ31" s="171"/>
       <c r="AK31" s="172"/>
     </row>
-    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -7505,7 +7497,7 @@
       <c r="AJ32" s="177"/>
       <c r="AK32" s="178"/>
     </row>
-    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="170" t="s">
@@ -7548,7 +7540,7 @@
       <c r="AJ33" s="171"/>
       <c r="AK33" s="172"/>
     </row>
-    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="176"/>
@@ -7587,7 +7579,7 @@
       <c r="AJ34" s="177"/>
       <c r="AK34" s="178"/>
     </row>
-    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="170" t="s">
@@ -7630,7 +7622,7 @@
       <c r="AJ35" s="171"/>
       <c r="AK35" s="172"/>
     </row>
-    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="176"/>
@@ -7669,7 +7661,7 @@
       <c r="AJ36" s="177"/>
       <c r="AK36" s="178"/>
     </row>
-    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -7714,7 +7706,7 @@
       <c r="AJ37" s="171"/>
       <c r="AK37" s="172"/>
     </row>
-    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="173"/>
@@ -7753,7 +7745,7 @@
       <c r="AJ38" s="174"/>
       <c r="AK38" s="175"/>
     </row>
-    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="173"/>
@@ -7792,7 +7784,7 @@
       <c r="AJ39" s="174"/>
       <c r="AK39" s="175"/>
     </row>
-    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="176"/>
@@ -7831,7 +7823,7 @@
       <c r="AJ40" s="177"/>
       <c r="AK40" s="178"/>
     </row>
-    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="173" t="s">
@@ -7874,7 +7866,7 @@
       <c r="AJ41" s="171"/>
       <c r="AK41" s="172"/>
     </row>
-    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -7915,7 +7907,7 @@
       <c r="AJ42" s="174"/>
       <c r="AK42" s="175"/>
     </row>
-    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="176"/>
@@ -7954,7 +7946,7 @@
       <c r="AJ43" s="177"/>
       <c r="AK43" s="178"/>
     </row>
-    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="173" t="s">
@@ -7997,7 +7989,7 @@
       <c r="AJ44" s="174"/>
       <c r="AK44" s="175"/>
     </row>
-    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="C45" s="173"/>
@@ -8036,7 +8028,7 @@
       <c r="AJ45" s="174"/>
       <c r="AK45" s="175"/>
     </row>
-    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="61"/>
       <c r="B46" s="67"/>
       <c r="C46" s="179"/>
@@ -8075,7 +8067,7 @@
       <c r="AJ46" s="180"/>
       <c r="AK46" s="181"/>
     </row>
-    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="67"/>
       <c r="C47" s="48"/>
@@ -8114,7 +8106,7 @@
       <c r="AJ47" s="58"/>
       <c r="AK47" s="59"/>
     </row>
-    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="68"/>
       <c r="C48" s="48"/>
@@ -8153,7 +8145,7 @@
       <c r="AJ48" s="58"/>
       <c r="AK48" s="59"/>
     </row>
-    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -8194,7 +8186,7 @@
       <c r="AJ49" s="52"/>
       <c r="AK49" s="53"/>
     </row>
-    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="67"/>
       <c r="C50" s="54"/>
@@ -8233,7 +8225,7 @@
       <c r="AJ50" s="55"/>
       <c r="AK50" s="57"/>
     </row>
-    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="164"/>
@@ -8276,7 +8268,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="103"/>
@@ -8315,7 +8307,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="99" t="s">
@@ -8443,21 +8435,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004009F7-098D-EC46-84C2-07CF91A4DD18}">
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A33" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="1" width="2.6640625" style="6"/>
+    <col min="2" max="2" width="2.5546875" style="6" customWidth="1"/>
+    <col min="3" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -8534,7 +8526,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -8571,7 +8563,7 @@
       <c r="AJ2" s="8"/>
       <c r="AK2" s="9"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -8608,7 +8600,7 @@
       <c r="AJ3" s="8"/>
       <c r="AK3" s="9"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -8645,7 +8637,7 @@
       <c r="AJ4" s="8"/>
       <c r="AK4" s="9"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -8653,7 +8645,7 @@
       <c r="AK5" s="12"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -8690,7 +8682,7 @@
       <c r="AJ6" s="14"/>
       <c r="AK6" s="15"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -8727,11 +8719,11 @@
       <c r="AJ7" s="14"/>
       <c r="AK7" s="15"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -8768,7 +8760,7 @@
       <c r="AJ9" s="17"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -8805,7 +8797,7 @@
       <c r="AJ10" s="17"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -8842,11 +8834,11 @@
       <c r="AJ11" s="17"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -8883,7 +8875,7 @@
       <c r="AJ13" s="21"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -8920,7 +8912,7 @@
       <c r="AJ14" s="21"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -8957,7 +8949,7 @@
       <c r="AJ15" s="21"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -8994,7 +8986,7 @@
       <c r="AJ16" s="21"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -9031,15 +9023,15 @@
       <c r="AJ17" s="21"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -9076,7 +9068,7 @@
       <c r="AJ20" s="23"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -9113,15 +9105,15 @@
       <c r="AJ21" s="23"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -9158,7 +9150,7 @@
       <c r="AJ24" s="21"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -9199,13 +9191,13 @@
       <c r="AJ25" s="21"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
@@ -9244,7 +9236,7 @@
       <c r="AJ27" s="23"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -9283,25 +9275,25 @@
       <c r="AJ28" s="23"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -9309,31 +9301,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -9341,31 +9333,31 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -9373,7 +9365,7 @@
       <c r="C42" s="7"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
@@ -9412,7 +9404,7 @@
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
@@ -9451,12 +9443,12 @@
       <c r="AJ44" s="8"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="12"/>
     </row>
-    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="67"/>
       <c r="C46" s="10"/>
@@ -9483,7 +9475,7 @@
       <c r="AJ46" s="26"/>
       <c r="AK46" s="27"/>
     </row>
-    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="67"/>
       <c r="C47" s="28"/>
@@ -9520,7 +9512,7 @@
       <c r="AJ47" s="26"/>
       <c r="AK47" s="27"/>
     </row>
-    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="68"/>
       <c r="C48" s="10"/>
@@ -9547,7 +9539,7 @@
       <c r="AJ48" s="26"/>
       <c r="AK48" s="27"/>
     </row>
-    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -9588,7 +9580,7 @@
       <c r="AJ49" s="14"/>
       <c r="AK49" s="15"/>
     </row>
-    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="67"/>
       <c r="C50" s="30"/>
@@ -9627,7 +9619,7 @@
       <c r="AJ50" s="33"/>
       <c r="AK50" s="34"/>
     </row>
-    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="164"/>
@@ -9670,7 +9662,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="103"/>
@@ -9709,7 +9701,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="99" t="s">
@@ -9805,20 +9797,20 @@
   <dimension ref="A1:BW53"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6"/>
-    <col min="76" max="16384" width="2.7109375" style="5"/>
+    <col min="1" max="1" width="2.6640625" style="6"/>
+    <col min="2" max="2" width="2.6640625" style="6" customWidth="1"/>
+    <col min="3" max="15" width="2.6640625" style="6"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6"/>
+    <col min="76" max="16384" width="2.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -9895,7 +9887,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -9932,7 +9924,7 @@
       <c r="AJ2" s="8"/>
       <c r="AK2" s="9"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -9969,7 +9961,7 @@
       <c r="AJ3" s="8"/>
       <c r="AK3" s="9"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -10006,7 +9998,7 @@
       <c r="AJ4" s="8"/>
       <c r="AK4" s="9"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -10014,7 +10006,7 @@
       <c r="AK5" s="12"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -10051,7 +10043,7 @@
       <c r="AJ6" s="14"/>
       <c r="AK6" s="15"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -10088,11 +10080,11 @@
       <c r="AJ7" s="14"/>
       <c r="AK7" s="15"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -10129,7 +10121,7 @@
       <c r="AJ9" s="17"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -10166,7 +10158,7 @@
       <c r="AJ10" s="17"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -10203,11 +10195,11 @@
       <c r="AJ11" s="17"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -10244,7 +10236,7 @@
       <c r="AJ13" s="21"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -10281,7 +10273,7 @@
       <c r="AJ14" s="21"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -10318,7 +10310,7 @@
       <c r="AJ15" s="21"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -10355,7 +10347,7 @@
       <c r="AJ16" s="21"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -10392,15 +10384,15 @@
       <c r="AJ17" s="21"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -10437,7 +10429,7 @@
       <c r="AJ20" s="23"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -10474,15 +10466,15 @@
       <c r="AJ21" s="23"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -10519,7 +10511,7 @@
       <c r="AJ24" s="21"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -10560,13 +10552,13 @@
       <c r="AJ25" s="21"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
@@ -10605,7 +10597,7 @@
       <c r="AJ27" s="23"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -10644,25 +10636,25 @@
       <c r="AJ28" s="23"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -10670,31 +10662,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -10702,13 +10694,13 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
@@ -10743,7 +10735,7 @@
       <c r="AG39" s="25"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
@@ -10778,7 +10770,7 @@
       <c r="AG40" s="25"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
@@ -10813,7 +10805,7 @@
       <c r="AG41" s="25"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -10850,7 +10842,7 @@
       <c r="AG42" s="25"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
@@ -10889,7 +10881,7 @@
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
@@ -10928,12 +10920,12 @@
       <c r="AJ44" s="8"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="24"/>
     </row>
-    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="64"/>
       <c r="C46" s="100"/>
@@ -10974,7 +10966,7 @@
       <c r="AJ46" s="106"/>
       <c r="AK46" s="107"/>
     </row>
-    <row r="47" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="61"/>
       <c r="B47" s="64"/>
       <c r="C47" s="96"/>
@@ -11013,7 +11005,7 @@
       <c r="AJ47" s="109"/>
       <c r="AK47" s="110"/>
     </row>
-    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="65"/>
       <c r="C48" s="99" t="s">
@@ -11064,7 +11056,7 @@
       <c r="AJ48" s="112"/>
       <c r="AK48" s="113"/>
     </row>
-    <row r="49" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -11119,7 +11111,7 @@
       <c r="AJ49" s="137"/>
       <c r="AK49" s="138"/>
     </row>
-    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="61"/>
       <c r="B50" s="64"/>
       <c r="C50" s="120"/>
@@ -11160,7 +11152,7 @@
       <c r="AJ50" s="115"/>
       <c r="AK50" s="116"/>
     </row>
-    <row r="51" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="120"/>
@@ -11199,7 +11191,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="120" t="s">
@@ -11246,7 +11238,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="144" t="s">
@@ -11363,21 +11355,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A799A7-5474-4EE0-88FB-BF028C29C22B}">
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A29" zoomScale="145" zoomScaleNormal="175" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A29" zoomScale="145" zoomScaleNormal="175" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" style="6" customWidth="1"/>
-    <col min="3" max="15" width="2.7109375" style="6" customWidth="1"/>
-    <col min="16" max="17" width="2.85546875" style="6" customWidth="1"/>
-    <col min="18" max="75" width="2.7109375" style="6" customWidth="1"/>
-    <col min="76" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="15" width="2.6640625" style="6" customWidth="1"/>
+    <col min="16" max="17" width="2.88671875" style="6" customWidth="1"/>
+    <col min="18" max="75" width="2.6640625" style="6" customWidth="1"/>
+    <col min="76" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -11454,7 +11444,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -11491,7 +11481,7 @@
       <c r="AJ2" s="8"/>
       <c r="AK2" s="9"/>
     </row>
-    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -11528,7 +11518,7 @@
       <c r="AJ3" s="8"/>
       <c r="AK3" s="9"/>
     </row>
-    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -11565,7 +11555,7 @@
       <c r="AJ4" s="8"/>
       <c r="AK4" s="9"/>
     </row>
-    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -11573,7 +11563,7 @@
       <c r="AK5" s="12"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -11610,7 +11600,7 @@
       <c r="AJ6" s="14"/>
       <c r="AK6" s="15"/>
     </row>
-    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -11647,11 +11637,11 @@
       <c r="AJ7" s="14"/>
       <c r="AK7" s="15"/>
     </row>
-    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="AK8" s="12"/>
     </row>
-    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -11688,7 +11678,7 @@
       <c r="AJ9" s="17"/>
       <c r="AK9" s="12"/>
     </row>
-    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -11725,7 +11715,7 @@
       <c r="AJ10" s="17"/>
       <c r="AK10" s="19"/>
     </row>
-    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -11762,11 +11752,11 @@
       <c r="AJ11" s="17"/>
       <c r="AK11" s="19"/>
     </row>
-    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="AK12" s="19"/>
     </row>
-    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -11803,7 +11793,7 @@
       <c r="AJ13" s="21"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -11840,7 +11830,7 @@
       <c r="AJ14" s="21"/>
       <c r="AK14" s="22"/>
     </row>
-    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -11877,7 +11867,7 @@
       <c r="AJ15" s="21"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -11914,7 +11904,7 @@
       <c r="AJ16" s="21"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -11951,15 +11941,15 @@
       <c r="AJ17" s="21"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -11996,7 +11986,7 @@
       <c r="AJ20" s="23"/>
       <c r="AK20" s="12"/>
     </row>
-    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -12033,15 +12023,15 @@
       <c r="AJ21" s="23"/>
       <c r="AK21" s="12"/>
     </row>
-    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="AK22" s="12"/>
     </row>
-    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="AK23" s="12"/>
     </row>
-    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" s="6" customFormat="1" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -12078,7 +12068,7 @@
       <c r="AJ24" s="21"/>
       <c r="AK24" s="12"/>
     </row>
-    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
@@ -12119,13 +12109,13 @@
       <c r="AJ25" s="21"/>
       <c r="AK25" s="12"/>
     </row>
-    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
       <c r="B26" s="64"/>
       <c r="C26" s="10"/>
       <c r="AK26" s="12"/>
     </row>
-    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" s="64"/>
       <c r="C27" s="10"/>
@@ -12164,7 +12154,7 @@
       <c r="AJ27" s="23"/>
       <c r="AK27" s="12"/>
     </row>
-    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="64"/>
       <c r="C28" s="10"/>
@@ -12203,25 +12193,25 @@
       <c r="AJ28" s="23"/>
       <c r="AK28" s="12"/>
     </row>
-    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="64"/>
       <c r="C29" s="10"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="64"/>
       <c r="C30" s="10"/>
       <c r="AK30" s="12"/>
     </row>
-    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="62"/>
       <c r="B31" s="65"/>
       <c r="C31" s="10"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>10</v>
       </c>
@@ -12229,31 +12219,31 @@
       <c r="C32" s="10"/>
       <c r="AK32" s="12"/>
     </row>
-    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="64"/>
       <c r="C33" s="10"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="64"/>
       <c r="C34" s="10"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="64"/>
       <c r="C35" s="10"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="62"/>
       <c r="B36" s="65"/>
       <c r="C36" s="10"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>9</v>
       </c>
@@ -12261,31 +12251,31 @@
       <c r="C37" s="10"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
       <c r="B38" s="64"/>
       <c r="C38" s="10"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
       <c r="B39" s="64"/>
       <c r="C39" s="10"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40" s="64"/>
       <c r="C40" s="10"/>
       <c r="AK40" s="12"/>
     </row>
-    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="B41" s="65"/>
       <c r="C41" s="7"/>
       <c r="AK41" s="9"/>
     </row>
-    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>8</v>
       </c>
@@ -12293,7 +12283,7 @@
       <c r="C42" s="7"/>
       <c r="AK42" s="9"/>
     </row>
-    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="64"/>
       <c r="C43" s="10"/>
@@ -12332,7 +12322,7 @@
       <c r="AJ43" s="8"/>
       <c r="AK43" s="9"/>
     </row>
-    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="61"/>
       <c r="B44" s="64"/>
       <c r="C44" s="10"/>
@@ -12371,12 +12361,12 @@
       <c r="AJ44" s="8"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="64"/>
       <c r="AK45" s="12"/>
     </row>
-    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="67"/>
       <c r="C46" s="10"/>
@@ -12403,7 +12393,7 @@
       <c r="AJ46" s="26"/>
       <c r="AK46" s="27"/>
     </row>
-    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="67"/>
       <c r="C47" s="28"/>
@@ -12440,7 +12430,7 @@
       <c r="AJ47" s="26"/>
       <c r="AK47" s="27"/>
     </row>
-    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="68"/>
       <c r="C48" s="10"/>
@@ -12467,7 +12457,7 @@
       <c r="AJ48" s="26"/>
       <c r="AK48" s="27"/>
     </row>
-    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>7</v>
       </c>
@@ -12508,7 +12498,7 @@
       <c r="AJ49" s="14"/>
       <c r="AK49" s="15"/>
     </row>
-    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="67"/>
       <c r="C50" s="30"/>
@@ -12547,7 +12537,7 @@
       <c r="AJ50" s="33"/>
       <c r="AK50" s="34"/>
     </row>
-    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="61"/>
       <c r="B51" s="64"/>
       <c r="C51" s="164"/>
@@ -12590,7 +12580,7 @@
       <c r="AJ51" s="118"/>
       <c r="AK51" s="119"/>
     </row>
-    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="61"/>
       <c r="B52" s="64"/>
       <c r="C52" s="103"/>
@@ -12629,7 +12619,7 @@
       <c r="AJ52" s="129"/>
       <c r="AK52" s="130"/>
     </row>
-    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62"/>
       <c r="B53" s="65"/>
       <c r="C53" s="99" t="s">

</xml_diff>